<commit_message>
[add]: deviation values are added
</commit_message>
<xml_diff>
--- a/PREVIOUS WORK/PART B- SALT WORK/MODEL 1/Model 1 Phase diagram/n=3/Li2SO4 -Model 1 n=3/Li2SO4 Model 1 n=3.xlsx
+++ b/PREVIOUS WORK/PART B- SALT WORK/MODEL 1/Model 1 Phase diagram/n=3/Li2SO4 -Model 1 n=3/Li2SO4 Model 1 n=3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Model 1\Model 1 Phase diagram\n=3\Li2SO4 -Model 1 n=3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://jda365-my.sharepoint.com/personal/dhanush_tamilselvan_jda_com/Documents/Desktop/Final-Year-Project/PREVIOUS WORK/PART B- SALT WORK/MODEL 1/Model 1 Phase diagram/n=3/Li2SO4 -Model 1 n=3/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91B05A73-5EA1-4EF8-8313-1A9F84350F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{70D051D8-7FC4-4B36-8B83-339629C5CAA1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{70D051D8-7FC4-4B36-8B83-339629C5CAA1}"/>
   </bookViews>
   <sheets>
     <sheet name="Literature" sheetId="1" r:id="rId1"/>
@@ -10420,9 +10420,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -10460,7 +10460,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -10566,7 +10566,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -10708,7 +10708,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -10718,16 +10718,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8463D1ED-08DA-4A8C-962D-FC3E5BA91019}">
   <dimension ref="A2:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="61.33203125" customWidth="1"/>
+    <col min="1" max="1" width="61.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -10735,7 +10735,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -10744,7 +10744,7 @@
         <v>55.555555555555557</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.39721750992497201</v>
       </c>
@@ -10756,7 +10756,7 @@
         <v>2.0999315560741503E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.77343371983886799</v>
       </c>
@@ -10768,7 +10768,7 @@
         <v>4.009100324751385E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.16501104717932</v>
       </c>
@@ -10780,7 +10780,7 @@
         <v>5.9187100732663596E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.53363414307117</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>7.6482269457726487E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1.9480782571690001</v>
       </c>
@@ -10804,7 +10804,7 @@
         <v>9.5183301773118539E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2.5775780152386898</v>
       </c>
@@ -10816,7 +10816,7 @@
         <v>0.12218269911280236</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3.0379743145793601</v>
       </c>
@@ -10828,7 +10828,7 @@
         <v>0.14093082479144514</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3.40650996577997</v>
       </c>
@@ -10840,7 +10840,7 @@
         <v>0.15537083421440145</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3.4067285775080598</v>
       </c>
@@ -10852,7 +10852,7 @@
         <v>0.15537925582263779</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>3.3837743460594498</v>
       </c>
@@ -10864,7 +10864,7 @@
         <v>0.15449406904479593</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>3.3917609611920398</v>
       </c>
@@ -10876,7 +10876,7 @@
         <v>0.15480226823819804</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>3.3535767793537201</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>0.1533267267576309</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3.3385654406920899</v>
       </c>
@@ -10900,7 +10900,7 @@
         <v>0.15274523568297013</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>3.31582982097156</v>
       </c>
@@ -10912,7 +10912,7 @@
         <v>0.1518630082022864</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.2397675137142401</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>0.14889810295327691</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.19425255192757</v>
       </c>
@@ -10936,7 +10936,7 @@
         <v>0.14711399763595187</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.1486938677952798</v>
       </c>
@@ -10948,7 +10948,7 @@
         <v>0.14532067215920066</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>3.1108594647218899</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>0.14382565541793893</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>3.0881238450013702</v>
       </c>
@@ -10972,7 +10972,7 @@
         <v>0.14292474476345665</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.0655631146632998</v>
       </c>
@@ -10984,7 +10984,7 @@
         <v>0.14202888808345326</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3.0583635017518001</v>
       </c>
@@ -10996,7 +10996,7 @@
         <v>0.14174260668796504</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>3.0202667646047199</v>
       </c>
@@ -11008,7 +11008,7 @@
         <v>0.14022456349807511</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3.0051679812518501</v>
       </c>
@@ -11020,7 +11020,7 @@
         <v>0.13962143433393306</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2.9292805633769898</v>
       </c>
@@ -11032,7 +11032,7 @@
         <v>0.13657721019261368</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2.9146627258259099</v>
       </c>
@@ -11044,7 +11044,7 @@
         <v>0.13598833941624983</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2.8763473769507399</v>
       </c>
@@ -11056,7 +11056,7 @@
         <v>0.13444100986675767</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2.87752788028238</v>
       </c>
@@ -11068,7 +11068,7 @@
         <v>0.13448876613221616</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2.8470679795029601</v>
       </c>
@@ -11080,7 +11080,7 @@
         <v>0.13325484791941505</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2.8320129184957099</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>0.13264367338351149</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2.8323626972606402</v>
       </c>
@@ -11104,7 +11104,7 @@
         <v>0.13265788276539192</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2.7203023254458198</v>
       </c>
@@ -11116,7 +11116,7 @@
         <v>0.12808160798714385</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2.6928592665139299</v>
       </c>
@@ -11128,7 +11128,7 @@
         <v>0.12695352908259044</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2.7179996152433499</v>
       </c>
@@ -11154,12 +11154,12 @@
       <selection activeCell="C1" sqref="C1:D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -11173,7 +11173,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -11187,7 +11187,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -11201,7 +11201,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -11215,7 +11215,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -11229,7 +11229,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -11243,7 +11243,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -11257,7 +11257,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -11271,7 +11271,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -11285,7 +11285,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -11293,7 +11293,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -11309,7 +11309,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -11334,12 +11334,12 @@
       <selection activeCell="C1" sqref="C1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -11353,7 +11353,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -11367,7 +11367,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -11381,7 +11381,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -11395,7 +11395,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -11409,7 +11409,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -11423,7 +11423,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -11437,7 +11437,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -11479,7 +11479,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -11507,7 +11507,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -11521,7 +11521,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -11535,7 +11535,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -11549,7 +11549,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -11563,7 +11563,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -11577,7 +11577,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -11591,7 +11591,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -11605,7 +11605,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -11619,7 +11619,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -11633,7 +11633,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -11647,7 +11647,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -11661,7 +11661,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -11675,7 +11675,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -11689,7 +11689,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -11703,7 +11703,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -11717,7 +11717,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -11731,7 +11731,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -11745,7 +11745,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -11759,7 +11759,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -11773,7 +11773,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -11787,7 +11787,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -11801,7 +11801,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -11815,7 +11815,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -11829,7 +11829,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -11843,7 +11843,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -11857,7 +11857,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -11871,7 +11871,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -11885,7 +11885,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -11899,7 +11899,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -11913,7 +11913,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -11927,7 +11927,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -11941,7 +11941,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -11955,7 +11955,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -11969,7 +11969,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -12011,7 +12011,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -12025,7 +12025,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -12039,7 +12039,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -12053,7 +12053,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -12081,7 +12081,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -12095,7 +12095,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -12109,7 +12109,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -12123,7 +12123,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -12137,7 +12137,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -12151,7 +12151,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -12165,7 +12165,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -12179,7 +12179,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -12207,7 +12207,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -12221,7 +12221,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -12235,7 +12235,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -12249,7 +12249,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -12263,7 +12263,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -12277,7 +12277,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="15.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -12291,7 +12291,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -12305,7 +12305,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -12319,7 +12319,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -12333,7 +12333,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -12347,7 +12347,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -12361,7 +12361,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -12375,7 +12375,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -12389,7 +12389,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -12403,7 +12403,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -12417,7 +12417,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -12431,7 +12431,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -12445,7 +12445,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -12459,7 +12459,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -12473,7 +12473,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -12498,9 +12498,9 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>4.6649500000000003E-2</v>
       </c>
@@ -12508,7 +12508,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.14310999999999999</v>
       </c>
@@ -12516,7 +12516,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.13127800000000001</v>
       </c>
@@ -12524,7 +12524,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.11945500000000001</v>
       </c>
@@ -12532,7 +12532,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.10871400000000001</v>
       </c>
@@ -12540,7 +12540,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9.5834000000000003E-2</v>
       </c>
@@ -12548,7 +12548,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6.7374600000000007E-2</v>
       </c>
@@ -12556,7 +12556,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7.2246199999999997E-2</v>
       </c>
@@ -12564,7 +12564,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7.3763899999999993E-2</v>
       </c>
@@ -12572,7 +12572,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>6.8656999999999996E-2</v>
       </c>
@@ -12580,7 +12580,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>3.6262299999999997E-2</v>
       </c>
@@ -12588,7 +12588,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2.8831099999999998E-2</v>
       </c>
@@ -12596,7 +12596,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1.3312600000000001E-2</v>
       </c>
@@ -12604,7 +12604,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1.2612000000000001E-3</v>
       </c>
@@ -12612,7 +12612,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.156915</v>
       </c>
@@ -12620,7 +12620,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.14082900000000001</v>
       </c>
@@ -12628,7 +12628,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.15599499999999999</v>
       </c>
@@ -12636,7 +12636,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.15305199999999999</v>
       </c>
@@ -12644,7 +12644,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.120573</v>
       </c>
@@ -12652,7 +12652,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.15463099999999999</v>
       </c>
@@ -12660,7 +12660,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.15418100000000001</v>
       </c>
@@ -12668,7 +12668,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.15373400000000001</v>
       </c>
@@ -12676,7 +12676,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.149398</v>
       </c>
@@ -12684,7 +12684,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.15284700000000001</v>
       </c>
@@ -12692,7 +12692,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.15218899999999999</v>
       </c>
@@ -12700,7 +12700,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.157162</v>
       </c>
@@ -12708,7 +12708,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.103396</v>
       </c>
@@ -12716,7 +12716,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.15110499999999999</v>
       </c>
@@ -12724,7 +12724,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.15089</v>
       </c>
@@ -12732,7 +12732,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.126448</v>
       </c>
@@ -12740,7 +12740,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.15024999999999999</v>
       </c>
@@ -12748,7 +12748,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.14982699999999999</v>
       </c>
@@ -12756,7 +12756,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.149197</v>
       </c>
@@ -12764,7 +12764,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.127195</v>
       </c>
@@ -12772,7 +12772,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.148369</v>
       </c>
@@ -12780,7 +12780,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0.12831100000000001</v>
       </c>
@@ -12788,7 +12788,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.14795900000000001</v>
       </c>
@@ -12796,7 +12796,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>0.14755199999999999</v>
       </c>
@@ -12804,7 +12804,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>0.14735000000000001</v>
       </c>
@@ -12812,7 +12812,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>0.15626399999999999</v>
       </c>
@@ -12820,7 +12820,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0.10408199999999999</v>
       </c>
@@ -12828,7 +12828,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>0.14674799999999999</v>
       </c>
@@ -12836,7 +12836,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>0.14654900000000001</v>
       </c>
@@ -12844,7 +12844,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>0.145761</v>
       </c>
@@ -12852,7 +12852,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0.145179</v>
       </c>
@@ -12860,7 +12860,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>0.144986</v>
       </c>
@@ -12868,7 +12868,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>0.14479500000000001</v>
       </c>
@@ -12876,7 +12876,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>0.14946799999999999</v>
       </c>
@@ -12884,7 +12884,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>0.10672</v>
       </c>
@@ -12892,7 +12892,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>0.14310999999999999</v>
       </c>
@@ -12900,7 +12900,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.13169600000000001</v>
       </c>
@@ -12908,7 +12908,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>0.14274600000000001</v>
       </c>
@@ -12916,7 +12916,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>0.14132500000000001</v>
       </c>
@@ -12924,7 +12924,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>0.14080799999999999</v>
       </c>
@@ -12932,7 +12932,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>0.13592499999999999</v>
       </c>
@@ -12940,7 +12940,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>0.14046800000000001</v>
       </c>
@@ -12948,7 +12948,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>0.13509099999999999</v>
       </c>
@@ -12956,7 +12956,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>0.113954</v>
       </c>
@@ -12964,7 +12964,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>0.13930899999999999</v>
       </c>
@@ -12972,7 +12972,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>0.138987</v>
       </c>
@@ -12980,7 +12980,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>0.13866999999999999</v>
       </c>
@@ -12988,7 +12988,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>0.10288899999999999</v>
       </c>
@@ -12996,7 +12996,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>0.13820099999999999</v>
       </c>
@@ -13004,7 +13004,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>0.138047</v>
       </c>
@@ -13012,7 +13012,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>0.142458</v>
       </c>
@@ -13020,7 +13020,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>0.13744100000000001</v>
       </c>
@@ -13028,7 +13028,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>0.155553</v>
       </c>
@@ -13036,7 +13036,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>0.136709</v>
       </c>
@@ -13044,7 +13044,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>0.13656599999999999</v>
       </c>
@@ -13052,7 +13052,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>0.13614299999999999</v>
       </c>
@@ -13060,7 +13060,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>0.13586699999999999</v>
       </c>
@@ -13068,7 +13068,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>0.135329</v>
       </c>
@@ -13076,7 +13076,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>0.13480900000000001</v>
       </c>
@@ -13084,7 +13084,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>0.134682</v>
       </c>
@@ -13092,7 +13092,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>0.13455600000000001</v>
       </c>
@@ -13100,7 +13100,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>0.134432</v>
       </c>
@@ -13108,7 +13108,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>0.13430800000000001</v>
       </c>
@@ -13116,7 +13116,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>0.13362199999999999</v>
       </c>
@@ -13124,7 +13124,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>0.13394600000000001</v>
       </c>
@@ -13132,7 +13132,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>0.133827</v>
       </c>
@@ -13140,7 +13140,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>0.13347899999999999</v>
       </c>
@@ -13148,7 +13148,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>0.13325300000000001</v>
       </c>
@@ -13156,7 +13156,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>0.123907</v>
       </c>
@@ -13164,7 +13164,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>0.13303300000000001</v>
       </c>
@@ -13172,7 +13172,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>0.15268499999999999</v>
       </c>
@@ -13180,7 +13180,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>0.132711</v>
       </c>
@@ -13188,7 +13188,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>0.14449799999999999</v>
       </c>
@@ -13196,7 +13196,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>0.13240099999999999</v>
       </c>
@@ -13204,7 +13204,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>0.132301</v>
       </c>
@@ -13212,7 +13212,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>0.13200700000000001</v>
       </c>
@@ -13220,7 +13220,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>0.131911</v>
       </c>
@@ -13228,7 +13228,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>0.135736</v>
       </c>
@@ -13236,7 +13236,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>0.131633</v>
       </c>
@@ -13244,7 +13244,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>0.13154299999999999</v>
       </c>
@@ -13252,7 +13252,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>0.108525</v>
       </c>
@@ -13260,7 +13260,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>0.13119700000000001</v>
       </c>
@@ -13268,7 +13268,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>0.13111300000000001</v>
       </c>
@@ -13276,7 +13276,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>0.13103200000000001</v>
       </c>
@@ -13284,7 +13284,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>0.13095100000000001</v>
       </c>
@@ -13292,7 +13292,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>0.12748000000000001</v>
       </c>
@@ -13300,7 +13300,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>0.13079399999999999</v>
       </c>
@@ -13308,7 +13308,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>0.11256099999999999</v>
       </c>
@@ -13316,7 +13316,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>0.127164</v>
       </c>
@@ -13324,7 +13324,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>0.13042699999999999</v>
       </c>
@@ -13332,7 +13332,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>0.155525</v>
       </c>
@@ -13340,7 +13340,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>0.13348099999999999</v>
       </c>
@@ -13348,7 +13348,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>0.117093</v>
       </c>
@@ -13356,7 +13356,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>0.12042799999999999</v>
       </c>
@@ -13364,7 +13364,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>0.11963</v>
       </c>
@@ -13372,7 +13372,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>0.13080700000000001</v>
       </c>
@@ -13380,7 +13380,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>0.12964200000000001</v>
       </c>
@@ -13388,7 +13388,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>0.12959200000000001</v>
       </c>
@@ -13396,7 +13396,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>0.12936400000000001</v>
       </c>
@@ -13404,7 +13404,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>0.12917500000000001</v>
       </c>
@@ -13412,7 +13412,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>0.120763</v>
       </c>
@@ -13420,7 +13420,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>0.129</v>
       </c>
@@ -13428,7 +13428,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>0.12895400000000001</v>
       </c>
@@ -13436,7 +13436,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>0.12889700000000001</v>
       </c>
@@ -13444,7 +13444,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>0.153007</v>
       </c>
@@ -13452,7 +13452,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>0.12883500000000001</v>
       </c>
@@ -13460,7 +13460,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>0.128827</v>
       </c>
@@ -13468,7 +13468,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>0.12881699999999999</v>
       </c>
@@ -13476,7 +13476,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>0.12881500000000001</v>
       </c>
@@ -13484,7 +13484,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>0.12692200000000001</v>
       </c>
@@ -13492,7 +13492,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>0.124098</v>
       </c>
@@ -13500,7 +13500,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>0.12882099999999999</v>
       </c>
@@ -13508,7 +13508,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>0.115513</v>
       </c>
@@ -13516,7 +13516,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>0.12486800000000001</v>
       </c>
@@ -13524,7 +13524,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>0.11730599999999999</v>
       </c>
@@ -13532,7 +13532,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>0.12893499999999999</v>
       </c>
@@ -13540,7 +13540,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>0.12895699999999999</v>
       </c>
@@ -13548,7 +13548,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>0.12930800000000001</v>
       </c>
@@ -13556,7 +13556,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>0.147288</v>
       </c>
@@ -13564,7 +13564,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>0.11360199999999999</v>
       </c>
@@ -13572,7 +13572,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>0.103772</v>
       </c>
@@ -13580,7 +13580,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>0.12915499999999999</v>
       </c>
@@ -13588,7 +13588,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>7.1023000000000003E-2</v>
       </c>
@@ -13596,7 +13596,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>0.12939400000000001</v>
       </c>
@@ -13604,7 +13604,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>0.12944</v>
       </c>
@@ -13612,7 +13612,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>0.126083</v>
       </c>
@@ -13620,7 +13620,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>0.129939</v>
       </c>
@@ -13628,7 +13628,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>0.14154800000000001</v>
       </c>
@@ -13646,16 +13646,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C17770F-88A3-4FE5-B26C-1A055981A772}">
   <dimension ref="A1:B90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0.129939</v>
       </c>
@@ -13663,7 +13663,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0.12944</v>
       </c>
@@ -13671,7 +13671,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>0.12939400000000001</v>
       </c>
@@ -13679,7 +13679,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0.12915499999999999</v>
       </c>
@@ -13687,7 +13687,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>0.12930800000000001</v>
       </c>
@@ -13695,7 +13695,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>0.12895699999999999</v>
       </c>
@@ -13703,7 +13703,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>0.12893499999999999</v>
       </c>
@@ -13711,7 +13711,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0.12882099999999999</v>
       </c>
@@ -13719,7 +13719,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.12881500000000001</v>
       </c>
@@ -13727,7 +13727,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.12881699999999999</v>
       </c>
@@ -13735,7 +13735,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.128827</v>
       </c>
@@ -13743,7 +13743,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.12883500000000001</v>
       </c>
@@ -13751,7 +13751,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.12889700000000001</v>
       </c>
@@ -13759,7 +13759,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.12895400000000001</v>
       </c>
@@ -13767,7 +13767,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>0.129</v>
       </c>
@@ -13775,7 +13775,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>0.12917500000000001</v>
       </c>
@@ -13783,7 +13783,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>0.12936400000000001</v>
       </c>
@@ -13791,7 +13791,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>0.12959200000000001</v>
       </c>
@@ -13799,7 +13799,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>0.12964200000000001</v>
       </c>
@@ -13807,7 +13807,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>0.13042699999999999</v>
       </c>
@@ -13815,7 +13815,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0.13079399999999999</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>0.13095100000000001</v>
       </c>
@@ -13831,7 +13831,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0.13103200000000001</v>
       </c>
@@ -13839,7 +13839,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>0.13111300000000001</v>
       </c>
@@ -13847,7 +13847,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0.13119700000000001</v>
       </c>
@@ -13855,7 +13855,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>0.13154299999999999</v>
       </c>
@@ -13863,7 +13863,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>0.131633</v>
       </c>
@@ -13871,7 +13871,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>0.131911</v>
       </c>
@@ -13879,7 +13879,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>0.13200700000000001</v>
       </c>
@@ -13887,7 +13887,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>0.132301</v>
       </c>
@@ -13895,7 +13895,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>0.13240099999999999</v>
       </c>
@@ -13903,7 +13903,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>0.132711</v>
       </c>
@@ -13911,7 +13911,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>0.13303300000000001</v>
       </c>
@@ -13919,7 +13919,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>0.13325300000000001</v>
       </c>
@@ -13927,7 +13927,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>0.13347899999999999</v>
       </c>
@@ -13935,7 +13935,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>0.133827</v>
       </c>
@@ -13943,7 +13943,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>0.13394600000000001</v>
       </c>
@@ -13951,7 +13951,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>0.13362199999999999</v>
       </c>
@@ -13959,7 +13959,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>0.13430800000000001</v>
       </c>
@@ -13967,7 +13967,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>0.134432</v>
       </c>
@@ -13975,7 +13975,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>0.13455600000000001</v>
       </c>
@@ -13983,7 +13983,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>0.134682</v>
       </c>
@@ -13991,7 +13991,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>0.13480900000000001</v>
       </c>
@@ -13999,7 +13999,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>0.135329</v>
       </c>
@@ -14007,7 +14007,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>0.13586699999999999</v>
       </c>
@@ -14015,7 +14015,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>0.13614299999999999</v>
       </c>
@@ -14023,7 +14023,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>0.13656599999999999</v>
       </c>
@@ -14031,7 +14031,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>0.136709</v>
       </c>
@@ -14039,7 +14039,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>0.13744100000000001</v>
       </c>
@@ -14047,7 +14047,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>0.138047</v>
       </c>
@@ -14055,7 +14055,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>0.13820099999999999</v>
       </c>
@@ -14063,7 +14063,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>0.13866999999999999</v>
       </c>
@@ -14071,7 +14071,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>0.138987</v>
       </c>
@@ -14079,7 +14079,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>0.13930899999999999</v>
       </c>
@@ -14087,7 +14087,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>0.14046800000000001</v>
       </c>
@@ -14095,7 +14095,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>0.14080799999999999</v>
       </c>
@@ -14103,7 +14103,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.14132500000000001</v>
       </c>
@@ -14111,7 +14111,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>0.14274600000000001</v>
       </c>
@@ -14119,7 +14119,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>0.14310999999999999</v>
       </c>
@@ -14127,7 +14127,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>0.14479500000000001</v>
       </c>
@@ -14135,7 +14135,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>0.144986</v>
       </c>
@@ -14143,7 +14143,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>0.145179</v>
       </c>
@@ -14151,7 +14151,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>0.145761</v>
       </c>
@@ -14159,7 +14159,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>0.14654900000000001</v>
       </c>
@@ -14167,7 +14167,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>0.14674799999999999</v>
       </c>
@@ -14175,7 +14175,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>0.14735000000000001</v>
       </c>
@@ -14183,7 +14183,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>0.14755199999999999</v>
       </c>
@@ -14191,7 +14191,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>0.14795900000000001</v>
       </c>
@@ -14199,7 +14199,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>0.148369</v>
       </c>
@@ -14207,7 +14207,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>0.149197</v>
       </c>
@@ -14215,7 +14215,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>0.14982699999999999</v>
       </c>
@@ -14223,7 +14223,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>0.15024999999999999</v>
       </c>
@@ -14231,7 +14231,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>0.15089</v>
       </c>
@@ -14239,7 +14239,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>0.15110499999999999</v>
       </c>
@@ -14247,7 +14247,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>0.15218899999999999</v>
       </c>
@@ -14255,7 +14255,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>0.15284700000000001</v>
       </c>
@@ -14263,7 +14263,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>0.15373400000000001</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>0.15418100000000001</v>
       </c>
@@ -14279,7 +14279,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>0.15463099999999999</v>
       </c>
@@ -14287,7 +14287,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>0.15599499999999999</v>
       </c>
@@ -14295,7 +14295,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>0.156915</v>
       </c>
@@ -14303,7 +14303,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>0.14310999999999999</v>
       </c>
@@ -14311,7 +14311,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>0.13127800000000001</v>
       </c>
@@ -14319,7 +14319,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>0.11945500000000001</v>
       </c>
@@ -14327,7 +14327,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>0.10871400000000001</v>
       </c>
@@ -14335,7 +14335,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>9.5834000000000003E-2</v>
       </c>
@@ -14343,7 +14343,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>7.2246199999999997E-2</v>
       </c>
@@ -14351,7 +14351,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3.6262299999999997E-2</v>
       </c>
@@ -14359,7 +14359,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2.8831099999999998E-2</v>
       </c>
@@ -14367,7 +14367,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>1.3312600000000001E-2</v>
       </c>

</xml_diff>